<commit_message>
Experimental results will be retaken to deal with the phase shift error.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Datset/Dataset.xlsx
+++ b/Project/3501/Furkan/Datset/Dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Ölçüm Kurgusu</t>
   </si>
@@ -55,25 +55,28 @@
     <t>Trig Source (V25m)</t>
   </si>
   <si>
-    <t>Vds Bot (Pos) - H1</t>
-  </si>
-  <si>
-    <t>Vds Top(Neg) - H1</t>
-  </si>
-  <si>
     <t>Top - Turn - OFF</t>
   </si>
   <si>
-    <t>VdsTop (Pos) - H2</t>
-  </si>
-  <si>
-    <t>Vds Bot (Neg) - H2</t>
+    <t>Vds Bot (Pos) - H1 - 50</t>
+  </si>
+  <si>
+    <t>Vds Bot (Neg) - H2 -50</t>
+  </si>
+  <si>
+    <t>Vds Top(Neg) - H1 - 50</t>
+  </si>
+  <si>
+    <t>VdsTop (Pos) - H2 - 50</t>
+  </si>
+  <si>
+    <t>Vds Bot (Neg) - H2 - 50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,7 +415,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +459,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -476,10 +479,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -499,10 +502,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -519,13 +522,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>

</xml_diff>